<commit_message>
updates to fungi workup ss
</commit_message>
<xml_diff>
--- a/analyses/uwpr-apr2017/unipept-lca/231-peaks97-dno-nomods-lca.xlsx
+++ b/analyses/uwpr-apr2017/unipept-lca/231-peaks97-dno-nomods-lca.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/uwpr-apr2017/unipept-lca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B56E4-278E-6B46-840F-3409A749EA6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E028DC-0E8E-B743-BCD1-4AA1AF68C485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="231-peaks97-dno-nomods-lca" sheetId="1" r:id="rId1"/>
@@ -19551,7 +19551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1400" sqref="E1400"/>
     </sheetView>
   </sheetViews>
@@ -48589,8 +48589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AD6D6F-FC31-E249-B9D4-87F0E28E798E}">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AH27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>